<commit_message>
bom and report updated
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\UT\junior\ece-445l-lab-7-8-11-gam3769-cjh4858\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C01496-237C-4C91-95D0-38EE6620E739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57565829-EA3F-44B8-B4AB-F717AB14A544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -268,6 +268,27 @@
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/Broadcom-Avago/HLMP-4700?qs=jT9z6tsiFNlLY0m7YkBilg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/TE-Connectivity/2013499-1?qs=TL6PIybY3BOLK37GbUYdng%3D%3D</t>
+  </si>
+  <si>
+    <t>Micro USB to DIP</t>
+  </si>
+  <si>
+    <t>Adapter</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HiLetgo Micro USB to DIP Adapter 5pin Female PCB Converter </t>
+  </si>
+  <si>
+    <t>571-2013499-1</t>
+  </si>
+  <si>
+    <t>2013499-1</t>
   </si>
 </sst>
 </file>
@@ -820,7 +841,7 @@
   <dimension ref="A1:AMK106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -864,7 +885,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="7">
         <f>SUM(K6:K117)</f>
-        <v>36.760000000000005</v>
+        <v>42.660000000000004</v>
       </c>
       <c r="F2" s="8"/>
       <c r="H2" s="4"/>
@@ -1130,6 +1151,45 @@
       </c>
       <c r="M10" s="13" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="K11" s="2">
+        <f>J11*A11</f>
+        <v>5.8999999999999995</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="9:19" x14ac:dyDescent="0.3">
@@ -1435,9 +1495,10 @@
     <hyperlink ref="L8" r:id="rId4" xr:uid="{22621B91-298F-46C9-A17E-2AA19A14B9E6}"/>
     <hyperlink ref="M9" r:id="rId5" display="https://www.amazon.com/DSD-TECH-Adapter-FT232RL-Compatible/dp/B07BBPX8B8/ref=sr_1_13?crid=A9D59T3O8BG8&amp;dib=eyJ2IjoiMSJ9.d5vsloOHRmReaSnQwctqP9tvO_0mt6u7lTzaB3fuXMbmsHSDdRHgs-UzHTmsKlfMbwh-4wbUeL42Jx7xln4GQSH3TheG6t4Z4y1_HoKRrdQAG6L7_j-3xNeHFC-D31nAvrRVfsz3jhvWZRObJUjBbVkVyzM6rSMZMRG5fWdz27aan7AIQzKbl9l3pgEK02B9MhmyT253i5PIVPKU4leCXjWGqNNduZmavIdUDWIYGCA.DDnP_7dTZ9flCe_lJBsYkGayPRt9L9KJ6ga13HJbb34&amp;dib_tag=se&amp;keywords=ftdi+usb+to+serial&amp;qid=1710954063&amp;sprefix=ftdi%2Caps%2C179&amp;sr=8-13" xr:uid="{D8FEEA46-B090-4B1E-86D9-4D52A8BA3907}"/>
     <hyperlink ref="L9" r:id="rId6" xr:uid="{214F1DEC-3E66-4945-90A9-FD1570AD45EF}"/>
+    <hyperlink ref="M11" r:id="rId7" xr:uid="{4658D411-751F-4D94-AA69-EDE4D018DDEF}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>